<commit_message>
Fixed reviews parsing in BeautifulSoup
</commit_message>
<xml_diff>
--- a/templates/bs4_template.xlsx
+++ b/templates/bs4_template.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,7 +491,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Продавець: Rozetka.</t>
+          <t>Rozetka.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -511,67 +511,15 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Код:  395460480</t>
+          <t>395460480</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Відгуки  137</t>
+          <t>137</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
-        <is>
-          <t>Серія: iPhone 15, Стандарт зв'язку: 2G (GPRS/EDGE)3G (WCDMA/UMTS/HSPA)4G (LTE)5G, Діагональ екрана: 6.1, Роздільна здатність дисплея: 2556x1179, Тип матриці: OLED (Super Retina XDR)</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Мобільний телефон Apple iPhone 15 128GB Black (MTP03RX/A)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Black</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>128 ГБ</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Продавець: Rozetka.</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>33 999₴</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>37 999₴</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>https://content1.rozetka.com.ua/goods/images/medium/364623744.jpg, https://content2.rozetka.com.ua/goods/images/medium/364623745.jpg, https://content2.rozetka.com.ua/goods/images/medium/364623746.jpg, https://content.rozetka.com.ua/goods/images/medium/364761439.jpg, https://content.rozetka.com.ua/goods/images/medium/364761440.jpg, https://content2.rozetka.com.ua/goods/images/medium/364761441.jpg, https://content.rozetka.com.ua/goods/images/medium/364761442.jpg</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Код:  395460480</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Відгуки  137</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
         <is>
           <t>Серія: iPhone 15, Стандарт зв'язку: 2G (GPRS/EDGE)3G (WCDMA/UMTS/HSPA)4G (LTE)5G, Діагональ екрана: 6.1, Роздільна здатність дисплея: 2556x1179, Тип матриці: OLED (Super Retina XDR)</t>
         </is>

</xml_diff>